<commit_message>
DONE WITH CORRE OOPS done with corrections except for any more possible final ones from Bill, and I need to read it again and stuff.
</commit_message>
<xml_diff>
--- a/collection_efficiency.xlsx
+++ b/collection_efficiency.xlsx
@@ -448,7 +448,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,14 +526,14 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="1">
         <f>B1*B2*B3*B4*B5*B6*B7*B8*B9</f>
-        <v>4.7867820375374999E-3</v>
+        <v>4.4708544230600252E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -548,7 +548,7 @@
       </c>
       <c r="D10" s="1">
         <f>D9*B10</f>
-        <v>2.3933910187687499E-3</v>
+        <v>2.2354272115300126E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>